<commit_message>
Creacion de los .h
</commit_message>
<xml_diff>
--- a/genetico.xlsx
+++ b/genetico.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Castillo\Documents\MCTD\Segundo parcial\Actividad 10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/335edca88003ba7e/Escritorio/Proyecto_Metodos/MetodosCuantitativos/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_205EFB117F4DDAB0B3F371193B1CF9785A79408B" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -54,10 +55,19 @@
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -459,7 +469,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -599,28 +609,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -634,12 +626,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -660,17 +646,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -678,11 +670,29 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -718,7 +728,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1" descr="Recorte de pantalla"/>
+        <xdr:cNvPr id="2" name="Imagen 1" descr="Recorte de pantalla">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -761,7 +777,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2" descr="Recorte de pantalla"/>
+        <xdr:cNvPr id="3" name="Imagen 2" descr="Recorte de pantalla">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -804,7 +826,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Imagen 4" descr="Recorte de pantalla"/>
+        <xdr:cNvPr id="5" name="Imagen 4" descr="Recorte de pantalla">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -847,7 +875,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Imagen 5" descr="Recorte de pantalla"/>
+        <xdr:cNvPr id="6" name="Imagen 5" descr="Recorte de pantalla">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -890,7 +924,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Imagen 7" descr="Recorte de pantalla"/>
+        <xdr:cNvPr id="8" name="Imagen 7" descr="Recorte de pantalla">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -933,7 +973,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Imagen 8" descr="Recorte de pantalla"/>
+        <xdr:cNvPr id="9" name="Imagen 8" descr="Recorte de pantalla">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -976,7 +1022,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Imagen 10" descr="Recorte de pantalla"/>
+        <xdr:cNvPr id="11" name="Imagen 10" descr="Recorte de pantalla">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1020,7 +1072,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Imagen 12" descr="Recorte de pantalla"/>
+        <xdr:cNvPr id="13" name="Imagen 12" descr="Recorte de pantalla">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1064,7 +1122,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Imagen 13" descr="Recorte de pantalla"/>
+        <xdr:cNvPr id="14" name="Imagen 13" descr="Recorte de pantalla">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1107,7 +1171,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Imagen 14" descr="Recorte de pantalla"/>
+        <xdr:cNvPr id="15" name="Imagen 14" descr="Recorte de pantalla">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1150,7 +1220,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Imagen 17" descr="Recorte de pantalla"/>
+        <xdr:cNvPr id="18" name="Imagen 17" descr="Recorte de pantalla">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1194,7 +1270,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Imagen 18" descr="Recorte de pantalla"/>
+        <xdr:cNvPr id="19" name="Imagen 18" descr="Recorte de pantalla">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1237,7 +1319,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Imagen 22" descr="Recorte de pantalla"/>
+        <xdr:cNvPr id="23" name="Imagen 22" descr="Recorte de pantalla">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1281,7 +1369,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="Imagen 24" descr="Recorte de pantalla"/>
+        <xdr:cNvPr id="25" name="Imagen 24" descr="Recorte de pantalla">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1325,7 +1419,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="26" name="Imagen 25" descr="Recorte de pantalla"/>
+        <xdr:cNvPr id="26" name="Imagen 25" descr="Recorte de pantalla">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1369,7 +1469,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="27" name="Imagen 26" descr="Recorte de pantalla"/>
+        <xdr:cNvPr id="27" name="Imagen 26" descr="Recorte de pantalla">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1413,7 +1519,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="28" name="Imagen 27" descr="Recorte de pantalla"/>
+        <xdr:cNvPr id="28" name="Imagen 27" descr="Recorte de pantalla">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1462,7 +1574,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1" descr="Recorte de pantalla"/>
+        <xdr:cNvPr id="2" name="Imagen 1" descr="Recorte de pantalla">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1505,7 +1623,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2" descr="Recorte de pantalla"/>
+        <xdr:cNvPr id="3" name="Imagen 2" descr="Recorte de pantalla">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1548,7 +1672,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3" descr="Recorte de pantalla"/>
+        <xdr:cNvPr id="4" name="Imagen 3" descr="Recorte de pantalla">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1591,7 +1721,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Imagen 4" descr="Recorte de pantalla"/>
+        <xdr:cNvPr id="5" name="Imagen 4" descr="Recorte de pantalla">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1634,7 +1770,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Imagen 5" descr="Recorte de pantalla"/>
+        <xdr:cNvPr id="6" name="Imagen 5" descr="Recorte de pantalla">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1677,7 +1819,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Imagen 6" descr="Recorte de pantalla"/>
+        <xdr:cNvPr id="7" name="Imagen 6" descr="Recorte de pantalla">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1720,7 +1868,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Imagen 7" descr="Recorte de pantalla"/>
+        <xdr:cNvPr id="8" name="Imagen 7" descr="Recorte de pantalla">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1764,7 +1918,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Imagen 8" descr="Recorte de pantalla"/>
+        <xdr:cNvPr id="9" name="Imagen 8" descr="Recorte de pantalla">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2058,7 +2218,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A97" zoomScale="76" zoomScaleNormal="85" workbookViewId="0">
@@ -2213,64 +2373,64 @@
         <v>37</v>
       </c>
       <c r="B33" s="5">
-        <f ca="1">RAND()</f>
-        <v>0.32226731010817566</v>
+        <f t="shared" ref="B33:O33" ca="1" si="0">RAND()</f>
+        <v>0.23765027404885009</v>
       </c>
       <c r="C33" s="5">
-        <f ca="1">RAND()</f>
-        <v>0.56319837432050013</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.33180131346116493</v>
       </c>
       <c r="D33" s="5">
-        <f ca="1">RAND()</f>
-        <v>0.6507908258274735</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.18580626760806618</v>
       </c>
       <c r="E33" s="5">
-        <f ca="1">RAND()</f>
-        <v>0.88159348757937317</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.21464880547581666</v>
       </c>
       <c r="F33" s="5">
-        <f ca="1">RAND()</f>
-        <v>0.68139125479530116</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.93634645057411092</v>
       </c>
       <c r="G33" s="5">
-        <f ca="1">RAND()</f>
-        <v>0.77845838301038883</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.94085257848536574</v>
       </c>
       <c r="H33" s="5">
-        <f ca="1">RAND()</f>
-        <v>0.84111022260124535</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.19602314817158561</v>
       </c>
       <c r="I33" s="5">
-        <f ca="1">RAND()</f>
-        <v>2.3974561132641403E-3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.24426430555487688</v>
       </c>
       <c r="J33" s="5">
-        <f ca="1">RAND()</f>
-        <v>0.33834751126996176</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.61400391330095538</v>
       </c>
       <c r="K33" s="5">
-        <f ca="1">RAND()</f>
-        <v>0.48842735067358156</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.4423579579044397E-2</v>
       </c>
       <c r="L33" s="5">
-        <f ca="1">RAND()</f>
-        <v>0.32377589694126385</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.29401397151660691</v>
       </c>
       <c r="M33" s="5">
-        <f ca="1">RAND()</f>
-        <v>0.50561987079296944</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.61285577579415529</v>
       </c>
       <c r="N33" s="5">
-        <f ca="1">RAND()</f>
-        <v>0.51861985811492128</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.20114326256811632</v>
       </c>
       <c r="O33" s="5">
-        <f ca="1">RAND()</f>
-        <v>0.97945487302917045</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.1054508117837476</v>
       </c>
       <c r="P33" s="5">
-        <f t="shared" ref="P33" ca="1" si="0">RAND()</f>
-        <v>0.72088470611233402</v>
+        <f t="shared" ref="P33" ca="1" si="1">RAND()</f>
+        <v>0.74910758935047372</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.3">
@@ -2278,308 +2438,308 @@
         <v>29</v>
       </c>
       <c r="B34" s="5">
-        <f ca="1">RAND()</f>
-        <v>0.58330976335945517</v>
+        <f t="shared" ref="B34:N34" ca="1" si="2">RAND()</f>
+        <v>0.72236017947380615</v>
       </c>
       <c r="C34" s="5">
-        <f ca="1">RAND()</f>
-        <v>0.95840842574347274</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.15774320481166093</v>
       </c>
       <c r="D34" s="5">
-        <f ca="1">RAND()</f>
-        <v>0.16569964566349005</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.79623938206836231</v>
       </c>
       <c r="E34" s="5">
-        <f ca="1">RAND()</f>
-        <v>7.6867366370826917E-2</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.10143993033990917</v>
       </c>
       <c r="F34" s="5">
-        <f ca="1">RAND()</f>
-        <v>0.47585586634470212</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.12794731715018548</v>
       </c>
       <c r="G34" s="5">
-        <f ca="1">RAND()</f>
-        <v>0.82226509239864687</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.71988706897057098</v>
       </c>
       <c r="H34" s="5">
-        <f ca="1">RAND()</f>
-        <v>0.7210921623831209</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.91644816923144223</v>
       </c>
       <c r="I34" s="5">
-        <f ca="1">RAND()</f>
-        <v>0.23299642158423151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.60248626819447237</v>
       </c>
       <c r="J34" s="5">
-        <f ca="1">RAND()</f>
-        <v>0.64904618056401342</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.80043836572132232</v>
       </c>
       <c r="K34" s="5">
-        <f ca="1">RAND()</f>
-        <v>0.98807135979189786</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.60791069779881557</v>
       </c>
       <c r="L34" s="5">
-        <f ca="1">RAND()</f>
-        <v>0.49967392064822436</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.93694525181983346</v>
       </c>
       <c r="M34" s="5">
-        <f ca="1">RAND()</f>
-        <v>0.55539525829582348</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.8176414246453495</v>
       </c>
       <c r="N34" s="5">
-        <f ca="1">RAND()</f>
-        <v>0.74117009773435893</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.13982748641626408</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="7" t="s">
+      <c r="C36" s="35"/>
+      <c r="D36" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E36" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="F36" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G36" s="7" t="s">
+      <c r="G36" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H36" s="7" t="s">
+      <c r="H36" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I36" s="7" t="s">
+      <c r="I36" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J36" s="7" t="s">
+      <c r="J36" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="7">
+      <c r="C37" s="36"/>
+      <c r="D37" s="6">
         <f>D45</f>
         <v>2173</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="6">
         <f>E45</f>
         <v>773</v>
       </c>
-      <c r="F37" s="7" t="str">
+      <c r="F37" s="6" t="str">
         <f>IF(0.1*D37+0.6*E37&lt;=2000,"T","F")</f>
         <v>T</v>
       </c>
-      <c r="G37" s="7" t="str">
+      <c r="G37" s="6" t="str">
         <f>IF(D37+E37&lt;=6000,"T","F")</f>
         <v>T</v>
       </c>
-      <c r="H37" s="7" t="str">
+      <c r="H37" s="6" t="str">
         <f>IF(D37&lt;=4000,"T","F")</f>
         <v>T</v>
       </c>
-      <c r="I37" s="7" t="str">
+      <c r="I37" s="6" t="str">
         <f>IF(D37&gt;=0,"T","F")</f>
         <v>T</v>
       </c>
-      <c r="J37" s="7" t="str">
+      <c r="J37" s="6" t="str">
         <f>IF(E37&gt;=0,"T","F")</f>
         <v>T</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="7">
-        <f t="shared" ref="D38:E38" si="1">D46</f>
+      <c r="C38" s="36"/>
+      <c r="D38" s="6">
+        <f t="shared" ref="D38:E38" si="3">D46</f>
         <v>1546</v>
       </c>
-      <c r="E38" s="7">
-        <f t="shared" si="1"/>
+      <c r="E38" s="6">
+        <f t="shared" si="3"/>
         <v>1316</v>
       </c>
-      <c r="F38" s="7" t="str">
-        <f t="shared" ref="F38:F41" si="2">IF(0.1*D38+0.6*E38&lt;=2000,"T","F")</f>
-        <v>T</v>
-      </c>
-      <c r="G38" s="7" t="str">
-        <f t="shared" ref="G38:G41" si="3">IF(D38+E38&lt;=6000,"T","F")</f>
-        <v>T</v>
-      </c>
-      <c r="H38" s="7" t="str">
-        <f t="shared" ref="H38:H41" si="4">IF(D38&lt;=4000,"T","F")</f>
-        <v>T</v>
-      </c>
-      <c r="I38" s="7" t="str">
-        <f t="shared" ref="I38:I41" si="5">IF(D38&gt;=0,"T","F")</f>
-        <v>T</v>
-      </c>
-      <c r="J38" s="7" t="str">
-        <f t="shared" ref="J38:J41" si="6">IF(E38&gt;=0,"T","F")</f>
+      <c r="F38" s="6" t="str">
+        <f t="shared" ref="F38:F41" si="4">IF(0.1*D38+0.6*E38&lt;=2000,"T","F")</f>
+        <v>T</v>
+      </c>
+      <c r="G38" s="6" t="str">
+        <f t="shared" ref="G38:G41" si="5">IF(D38+E38&lt;=6000,"T","F")</f>
+        <v>T</v>
+      </c>
+      <c r="H38" s="6" t="str">
+        <f t="shared" ref="H38:H41" si="6">IF(D38&lt;=4000,"T","F")</f>
+        <v>T</v>
+      </c>
+      <c r="I38" s="6" t="str">
+        <f t="shared" ref="I38:I41" si="7">IF(D38&gt;=0,"T","F")</f>
+        <v>T</v>
+      </c>
+      <c r="J38" s="6" t="str">
+        <f t="shared" ref="J38:J41" si="8">IF(E38&gt;=0,"T","F")</f>
         <v>T</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="9"/>
-      <c r="D39" s="7">
-        <f t="shared" ref="D39:E39" si="7">D47</f>
+      <c r="C39" s="36"/>
+      <c r="D39" s="6">
+        <f t="shared" ref="D39:E39" si="9">D47</f>
         <v>2124</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E39" s="6">
+        <f t="shared" si="9"/>
+        <v>2235</v>
+      </c>
+      <c r="F39" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>T</v>
+      </c>
+      <c r="G39" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>T</v>
+      </c>
+      <c r="H39" s="6" t="str">
+        <f t="shared" si="6"/>
+        <v>T</v>
+      </c>
+      <c r="I39" s="6" t="str">
         <f t="shared" si="7"/>
-        <v>2235</v>
-      </c>
-      <c r="F39" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>T</v>
-      </c>
-      <c r="G39" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>T</v>
-      </c>
-      <c r="H39" s="7" t="str">
+        <v>T</v>
+      </c>
+      <c r="J39" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A40" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" s="37"/>
+      <c r="D40" s="6">
+        <f t="shared" ref="D40:E40" si="10">D48</f>
+        <v>3881</v>
+      </c>
+      <c r="E40" s="6">
+        <f t="shared" si="10"/>
+        <v>1859</v>
+      </c>
+      <c r="F40" s="6" t="str">
         <f t="shared" si="4"/>
         <v>T</v>
       </c>
-      <c r="I39" s="7" t="str">
+      <c r="G40" s="6" t="str">
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="J39" s="7" t="str">
+      <c r="H40" s="6" t="str">
         <f t="shared" si="6"/>
         <v>T</v>
       </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A40" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C40" s="10"/>
-      <c r="D40" s="7">
-        <f t="shared" ref="D40:E40" si="8">D48</f>
-        <v>3881</v>
-      </c>
-      <c r="E40" s="7">
+      <c r="I40" s="6" t="str">
+        <f t="shared" si="7"/>
+        <v>T</v>
+      </c>
+      <c r="J40" s="6" t="str">
         <f t="shared" si="8"/>
-        <v>1859</v>
-      </c>
-      <c r="F40" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>T</v>
-      </c>
-      <c r="G40" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>T</v>
-      </c>
-      <c r="H40" s="7" t="str">
+        <v>T</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="37"/>
+      <c r="D41" s="6">
+        <f t="shared" ref="D41:E41" si="11">D49</f>
+        <v>2720</v>
+      </c>
+      <c r="E41" s="6">
+        <f t="shared" si="11"/>
+        <v>2221</v>
+      </c>
+      <c r="F41" s="6" t="str">
         <f t="shared" si="4"/>
         <v>T</v>
       </c>
-      <c r="I40" s="7" t="str">
+      <c r="G41" s="6" t="str">
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="J40" s="7" t="str">
+      <c r="H41" s="6" t="str">
         <f t="shared" si="6"/>
         <v>T</v>
       </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A41" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C41" s="10"/>
-      <c r="D41" s="7">
-        <f t="shared" ref="D41:E41" si="9">D49</f>
-        <v>2720</v>
-      </c>
-      <c r="E41" s="7">
-        <f t="shared" si="9"/>
-        <v>2221</v>
-      </c>
-      <c r="F41" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>T</v>
-      </c>
-      <c r="G41" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>T</v>
-      </c>
-      <c r="H41" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>T</v>
-      </c>
-      <c r="I41" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>T</v>
-      </c>
-      <c r="J41" s="7" t="str">
-        <f t="shared" si="6"/>
+      <c r="I41" s="6" t="str">
+        <f t="shared" si="7"/>
+        <v>T</v>
+      </c>
+      <c r="J41" s="6" t="str">
+        <f t="shared" si="8"/>
         <v>T</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6" t="s">
+      <c r="C43" s="35"/>
+      <c r="D43" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E43" s="6"/>
+      <c r="E43" s="35"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="E44" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B45" s="8" t="s">
+      <c r="B45" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C45" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D45" s="7">
+      <c r="D45" s="6">
         <v>2173</v>
       </c>
-      <c r="E45" s="7">
+      <c r="E45" s="6">
         <v>773</v>
       </c>
       <c r="G45" s="4"/>
@@ -2599,16 +2759,16 @@
       <c r="U45" s="4"/>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B46" s="8" t="s">
+      <c r="B46" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D46" s="7">
+      <c r="D46" s="6">
         <v>1546</v>
       </c>
-      <c r="E46" s="7">
+      <c r="E46" s="6">
         <v>1316</v>
       </c>
       <c r="G46" s="4"/>
@@ -2628,44 +2788,44 @@
       <c r="U46" s="4"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D47" s="7">
+      <c r="D47" s="6">
         <v>2124</v>
       </c>
-      <c r="E47" s="7">
+      <c r="E47" s="6">
         <v>2235</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B48" s="8" t="s">
+      <c r="B48" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C48" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D48" s="7">
+      <c r="D48" s="6">
         <v>3881</v>
       </c>
-      <c r="E48" s="7">
+      <c r="E48" s="6">
         <v>1859</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C49" s="8" t="s">
+      <c r="C49" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D49" s="7">
+      <c r="D49" s="6">
         <v>2720</v>
       </c>
-      <c r="E49" s="7">
+      <c r="E49" s="6">
         <v>2221</v>
       </c>
     </row>
@@ -2675,205 +2835,205 @@
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A53" s="11" t="s">
+      <c r="A53" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B53" s="13" t="s">
+      <c r="B53" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="C53" s="14"/>
-      <c r="D53" s="7" t="s">
+      <c r="C53" s="27"/>
+      <c r="D53" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E53" s="7" t="s">
+      <c r="E53" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F53" s="15" t="s">
+      <c r="F53" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="G53" s="15" t="s">
+      <c r="G53" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="H53" s="15" t="s">
+      <c r="H53" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="I53" s="15" t="s">
+      <c r="I53" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="J53" s="15" t="s">
+      <c r="J53" s="9" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A54" s="11" t="s">
+      <c r="A54" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B54" s="13" t="s">
+      <c r="B54" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="C54" s="14"/>
-      <c r="D54" s="11">
+      <c r="C54" s="27"/>
+      <c r="D54" s="8">
         <v>2173</v>
       </c>
-      <c r="E54" s="11">
+      <c r="E54" s="8">
         <v>773</v>
       </c>
-      <c r="F54" s="16">
+      <c r="F54" s="10">
         <f>0.2*D54+0.5*E54</f>
         <v>821.1</v>
       </c>
-      <c r="G54" s="16">
+      <c r="G54" s="10">
         <f>F54/F59</f>
         <v>0.12272075088180785</v>
       </c>
-      <c r="H54" s="16">
+      <c r="H54" s="10">
         <f>G54</f>
         <v>0.12272075088180785</v>
       </c>
-      <c r="I54" s="16">
+      <c r="I54" s="10">
         <v>0.33749315660598289</v>
       </c>
-      <c r="J54" s="7" t="s">
+      <c r="J54" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B55" s="13" t="s">
+      <c r="B55" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="C55" s="14"/>
-      <c r="D55" s="11">
+      <c r="C55" s="27"/>
+      <c r="D55" s="8">
         <v>1546</v>
       </c>
-      <c r="E55" s="11">
+      <c r="E55" s="8">
         <v>1316</v>
       </c>
-      <c r="F55" s="16">
-        <f t="shared" ref="F55:F58" si="10">0.2*D55+0.5*E55</f>
+      <c r="F55" s="10">
+        <f t="shared" ref="F55:F58" si="12">0.2*D55+0.5*E55</f>
         <v>967.2</v>
       </c>
-      <c r="G55" s="16">
+      <c r="G55" s="10">
         <f>F55/F59</f>
         <v>0.14455670472888146</v>
       </c>
-      <c r="H55" s="16">
+      <c r="H55" s="10">
         <f>H54+G55</f>
         <v>0.26727745561068933</v>
       </c>
-      <c r="I55" s="16">
+      <c r="I55" s="10">
         <v>0.82202241638038787</v>
       </c>
-      <c r="J55" s="7" t="s">
+      <c r="J55" s="6" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A56" s="11" t="s">
+      <c r="A56" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B56" s="13" t="s">
+      <c r="B56" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C56" s="14"/>
-      <c r="D56" s="11">
+      <c r="C56" s="27"/>
+      <c r="D56" s="8">
         <v>2124</v>
       </c>
-      <c r="E56" s="11">
+      <c r="E56" s="8">
         <v>2235</v>
       </c>
-      <c r="F56" s="16">
-        <f t="shared" si="10"/>
+      <c r="F56" s="10">
+        <f t="shared" si="12"/>
         <v>1542.3</v>
       </c>
-      <c r="G56" s="16">
+      <c r="G56" s="10">
         <f>F56/F59</f>
         <v>0.23051055180247504</v>
       </c>
-      <c r="H56" s="16">
+      <c r="H56" s="10">
         <f>H55+G56</f>
         <v>0.49778800741316437</v>
       </c>
-      <c r="I56" s="16">
+      <c r="I56" s="10">
         <v>0.96074698967936412</v>
       </c>
-      <c r="J56" s="7" t="s">
+      <c r="J56" s="6" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A57" s="11" t="s">
+      <c r="A57" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B57" s="13" t="s">
+      <c r="B57" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="C57" s="14"/>
-      <c r="D57" s="11">
+      <c r="C57" s="27"/>
+      <c r="D57" s="8">
         <v>3881</v>
       </c>
-      <c r="E57" s="11">
+      <c r="E57" s="8">
         <v>1859</v>
       </c>
-      <c r="F57" s="16">
-        <f t="shared" si="10"/>
+      <c r="F57" s="10">
+        <f t="shared" si="12"/>
         <v>1705.7</v>
       </c>
-      <c r="G57" s="16">
+      <c r="G57" s="10">
         <f>F57/F59</f>
         <v>0.25493214563280925</v>
       </c>
-      <c r="H57" s="16">
+      <c r="H57" s="10">
         <f>H56+G57</f>
         <v>0.75272015304597362</v>
       </c>
-      <c r="I57" s="16">
+      <c r="I57" s="10">
         <v>0.64046149683610454</v>
       </c>
-      <c r="J57" s="7" t="s">
+      <c r="J57" s="6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A58" s="11" t="s">
+      <c r="A58" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B58" s="13" t="s">
+      <c r="B58" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="C58" s="14"/>
-      <c r="D58" s="11">
+      <c r="C58" s="27"/>
+      <c r="D58" s="8">
         <v>2720</v>
       </c>
-      <c r="E58" s="11">
+      <c r="E58" s="8">
         <v>2221</v>
       </c>
-      <c r="F58" s="16">
-        <f t="shared" si="10"/>
+      <c r="F58" s="10">
+        <f t="shared" si="12"/>
         <v>1654.5</v>
       </c>
-      <c r="G58" s="16">
+      <c r="G58" s="10">
         <f>F58/F59</f>
         <v>0.24727984695402641</v>
       </c>
-      <c r="H58" s="16">
+      <c r="H58" s="10">
         <f>H57+G58</f>
         <v>1</v>
       </c>
-      <c r="I58" s="16">
+      <c r="I58" s="10">
         <v>0.72185902976368654</v>
       </c>
-      <c r="J58" s="7" t="s">
+      <c r="J58" s="6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E59" s="7" t="s">
+      <c r="E59" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F59" s="16">
+      <c r="F59" s="10">
         <f>SUM(F54:F58)</f>
         <v>6690.8</v>
       </c>
@@ -2884,375 +3044,375 @@
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A64" s="7" t="s">
+      <c r="A64" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B64" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C64" s="6"/>
-      <c r="D64" s="7" t="s">
+      <c r="C64" s="35"/>
+      <c r="D64" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E64" s="7" t="s">
+      <c r="E64" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F64" s="7" t="s">
+      <c r="F64" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G64" s="7" t="s">
+      <c r="G64" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H64" s="7" t="s">
+      <c r="H64" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I64" s="7" t="s">
+      <c r="I64" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J64" s="7" t="s">
+      <c r="J64" s="6" t="s">
         <v>28</v>
       </c>
       <c r="L64" t="s">
         <v>65</v>
       </c>
-      <c r="M64" s="18" t="s">
+      <c r="M64" s="12" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A65" s="7" t="s">
+      <c r="A65" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B65" s="19" t="s">
+      <c r="B65" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C65" s="14"/>
-      <c r="D65" s="11">
+      <c r="C65" s="27"/>
+      <c r="D65" s="8">
         <v>2124</v>
       </c>
-      <c r="E65" s="11">
+      <c r="E65" s="8">
         <v>2235</v>
       </c>
-      <c r="F65" s="7" t="str">
+      <c r="F65" s="6" t="str">
         <f>IF(0.1*D65+0.6*E65&lt;=2000,"T","F")</f>
         <v>T</v>
       </c>
-      <c r="G65" s="7" t="str">
+      <c r="G65" s="6" t="str">
         <f>IF(D65+E65&lt;=6000,"T","F")</f>
         <v>T</v>
       </c>
-      <c r="H65" s="7" t="str">
+      <c r="H65" s="6" t="str">
         <f>IF(D65&lt;=4000,"T","F")</f>
         <v>T</v>
       </c>
-      <c r="I65" s="7" t="str">
+      <c r="I65" s="6" t="str">
         <f>IF(D65&gt;=0,"T","F")</f>
         <v>T</v>
       </c>
-      <c r="J65" s="7" t="str">
+      <c r="J65" s="6" t="str">
         <f>IF(E65&gt;=0,"T","F")</f>
         <v>T</v>
       </c>
       <c r="L65" t="str">
         <f ca="1">IF(RAND()*10&gt;5,"Mutación","Cruce")</f>
-        <v>Mutación</v>
-      </c>
-      <c r="M65" s="17">
+        <v>Cruce</v>
+      </c>
+      <c r="M65" s="11">
         <f ca="1">RAND()*27</f>
-        <v>17.96885238195032</v>
+        <v>15.189139413849057</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A66" s="7" t="s">
+      <c r="A66" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B66" s="19" t="s">
+      <c r="B66" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="C66" s="14"/>
-      <c r="D66" s="11">
+      <c r="C66" s="27"/>
+      <c r="D66" s="8">
         <v>3881</v>
       </c>
-      <c r="E66" s="11">
+      <c r="E66" s="8">
         <v>1859</v>
       </c>
-      <c r="F66" s="7" t="str">
-        <f t="shared" ref="F66:F69" si="11">IF(0.1*D66+0.6*E66&lt;=2000,"T","F")</f>
-        <v>T</v>
-      </c>
-      <c r="G66" s="7" t="str">
-        <f t="shared" ref="G66:G69" si="12">IF(D66+E66&lt;=6000,"T","F")</f>
-        <v>T</v>
-      </c>
-      <c r="H66" s="7" t="str">
-        <f t="shared" ref="H66:H69" si="13">IF(D66&lt;=4000,"T","F")</f>
-        <v>T</v>
-      </c>
-      <c r="I66" s="7" t="str">
-        <f t="shared" ref="I66:I69" si="14">IF(D66&gt;=0,"T","F")</f>
-        <v>T</v>
-      </c>
-      <c r="J66" s="7" t="str">
-        <f t="shared" ref="J66:J69" si="15">IF(E66&gt;=0,"T","F")</f>
-        <v>T</v>
-      </c>
-      <c r="M66" s="17"/>
+      <c r="F66" s="6" t="str">
+        <f t="shared" ref="F66:F69" si="13">IF(0.1*D66+0.6*E66&lt;=2000,"T","F")</f>
+        <v>T</v>
+      </c>
+      <c r="G66" s="6" t="str">
+        <f t="shared" ref="G66:G69" si="14">IF(D66+E66&lt;=6000,"T","F")</f>
+        <v>T</v>
+      </c>
+      <c r="H66" s="6" t="str">
+        <f t="shared" ref="H66:H69" si="15">IF(D66&lt;=4000,"T","F")</f>
+        <v>T</v>
+      </c>
+      <c r="I66" s="6" t="str">
+        <f t="shared" ref="I66:I69" si="16">IF(D66&gt;=0,"T","F")</f>
+        <v>T</v>
+      </c>
+      <c r="J66" s="6" t="str">
+        <f t="shared" ref="J66:J69" si="17">IF(E66&gt;=0,"T","F")</f>
+        <v>T</v>
+      </c>
+      <c r="M66" s="11"/>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A67" s="7" t="s">
+      <c r="A67" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B67" s="19" t="s">
+      <c r="B67" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="C67" s="14"/>
-      <c r="D67" s="11">
+      <c r="C67" s="27"/>
+      <c r="D67" s="8">
         <v>2720</v>
       </c>
-      <c r="E67" s="11">
+      <c r="E67" s="8">
         <v>2221</v>
       </c>
-      <c r="F67" s="7" t="str">
-        <f t="shared" si="11"/>
-        <v>T</v>
-      </c>
-      <c r="G67" s="7" t="str">
-        <f t="shared" si="12"/>
-        <v>T</v>
-      </c>
-      <c r="H67" s="7" t="str">
+      <c r="F67" s="6" t="str">
         <f t="shared" si="13"/>
         <v>T</v>
       </c>
-      <c r="I67" s="7" t="str">
+      <c r="G67" s="6" t="str">
         <f t="shared" si="14"/>
         <v>T</v>
       </c>
-      <c r="J67" s="7" t="str">
+      <c r="H67" s="6" t="str">
         <f t="shared" si="15"/>
         <v>T</v>
       </c>
+      <c r="I67" s="6" t="str">
+        <f t="shared" si="16"/>
+        <v>T</v>
+      </c>
+      <c r="J67" s="6" t="str">
+        <f t="shared" si="17"/>
+        <v>T</v>
+      </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A68" s="7" t="s">
+      <c r="A68" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B68" s="19" t="s">
+      <c r="B68" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="C68" s="14"/>
-      <c r="D68" s="7">
-        <f t="shared" ref="D68:E68" si="16">D76</f>
+      <c r="C68" s="27"/>
+      <c r="D68" s="6">
+        <f t="shared" ref="D68:E68" si="18">D76</f>
         <v>2125</v>
       </c>
-      <c r="E68" s="7">
+      <c r="E68" s="6">
+        <f t="shared" si="18"/>
+        <v>1859</v>
+      </c>
+      <c r="F68" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>T</v>
+      </c>
+      <c r="G68" s="6" t="str">
+        <f t="shared" si="14"/>
+        <v>T</v>
+      </c>
+      <c r="H68" s="6" t="str">
+        <f t="shared" si="15"/>
+        <v>T</v>
+      </c>
+      <c r="I68" s="6" t="str">
         <f t="shared" si="16"/>
-        <v>1859</v>
-      </c>
-      <c r="F68" s="7" t="str">
-        <f t="shared" si="11"/>
-        <v>T</v>
-      </c>
-      <c r="G68" s="7" t="str">
-        <f t="shared" si="12"/>
-        <v>T</v>
-      </c>
-      <c r="H68" s="7" t="str">
+        <v>T</v>
+      </c>
+      <c r="J68" s="6" t="str">
+        <f t="shared" si="17"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A69" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B69" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C69" s="27"/>
+      <c r="D69" s="6">
+        <f t="shared" ref="D69:E69" si="19">D77</f>
+        <v>2720</v>
+      </c>
+      <c r="E69" s="6">
+        <f t="shared" si="19"/>
+        <v>2237</v>
+      </c>
+      <c r="F69" s="6" t="str">
         <f t="shared" si="13"/>
         <v>T</v>
       </c>
-      <c r="I68" s="7" t="str">
+      <c r="G69" s="6" t="str">
         <f t="shared" si="14"/>
         <v>T</v>
       </c>
-      <c r="J68" s="7" t="str">
+      <c r="H69" s="6" t="str">
         <f t="shared" si="15"/>
         <v>T</v>
       </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A69" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B69" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="C69" s="14"/>
-      <c r="D69" s="7">
-        <f t="shared" ref="D69:E69" si="17">D77</f>
-        <v>2720</v>
-      </c>
-      <c r="E69" s="7">
+      <c r="I69" s="6" t="str">
+        <f t="shared" si="16"/>
+        <v>T</v>
+      </c>
+      <c r="J69" s="6" t="str">
         <f t="shared" si="17"/>
-        <v>2237</v>
-      </c>
-      <c r="F69" s="7" t="str">
-        <f t="shared" si="11"/>
-        <v>T</v>
-      </c>
-      <c r="G69" s="7" t="str">
-        <f t="shared" si="12"/>
-        <v>T</v>
-      </c>
-      <c r="H69" s="7" t="str">
-        <f t="shared" si="13"/>
-        <v>T</v>
-      </c>
-      <c r="I69" s="7" t="str">
-        <f t="shared" si="14"/>
-        <v>T</v>
-      </c>
-      <c r="J69" s="7" t="str">
-        <f t="shared" si="15"/>
         <v>T</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B71" s="6" t="s">
+      <c r="B71" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C71" s="6"/>
-      <c r="D71" s="6" t="s">
+      <c r="C71" s="35"/>
+      <c r="D71" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E71" s="6"/>
-      <c r="F71" s="12" t="s">
+      <c r="E71" s="35"/>
+      <c r="F71" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="G71" s="12" t="s">
+      <c r="G71" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="H71" s="20" t="s">
+      <c r="H71" s="31" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B72" s="7" t="s">
+      <c r="B72" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C72" s="7" t="s">
+      <c r="C72" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D72" s="7" t="s">
+      <c r="D72" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E72" s="7" t="s">
+      <c r="E72" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F72" s="12"/>
-      <c r="G72" s="12"/>
-      <c r="H72" s="20"/>
+      <c r="F72" s="30"/>
+      <c r="G72" s="30"/>
+      <c r="H72" s="31"/>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B73" s="8" t="s">
+      <c r="B73" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C73" s="8" t="s">
+      <c r="C73" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D73" s="7">
+      <c r="D73" s="6">
         <v>2124</v>
       </c>
-      <c r="E73" s="7">
+      <c r="E73" s="6">
         <v>2235</v>
       </c>
-      <c r="F73" s="11" t="s">
+      <c r="F73" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="G73" s="21" t="s">
+      <c r="G73" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="H73" s="22"/>
+      <c r="H73" s="14"/>
       <c r="I73" s="4"/>
       <c r="J73" s="4"/>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B74" s="8" t="s">
+      <c r="B74" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C74" s="8" t="s">
+      <c r="C74" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D74" s="7">
+      <c r="D74" s="6">
         <v>3881</v>
       </c>
-      <c r="E74" s="7">
+      <c r="E74" s="6">
         <v>1859</v>
       </c>
-      <c r="F74" s="11" t="s">
+      <c r="F74" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="G74" s="21" t="s">
+      <c r="G74" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="H74" s="22"/>
+      <c r="H74" s="14"/>
       <c r="I74" s="4"/>
       <c r="J74" s="4"/>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B75" s="8" t="s">
+      <c r="B75" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C75" s="8" t="s">
+      <c r="C75" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D75" s="7">
+      <c r="D75" s="6">
         <v>2720</v>
       </c>
-      <c r="E75" s="7">
+      <c r="E75" s="6">
         <v>2221</v>
       </c>
-      <c r="F75" s="11" t="s">
+      <c r="F75" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="G75" s="11" t="s">
+      <c r="G75" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="H75" s="7"/>
+      <c r="H75" s="6"/>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B76" s="8" t="s">
+      <c r="B76" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C76" s="8" t="s">
+      <c r="C76" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D76" s="7">
+      <c r="D76" s="6">
         <v>2125</v>
       </c>
-      <c r="E76" s="7">
+      <c r="E76" s="6">
         <v>1859</v>
       </c>
-      <c r="F76" s="11" t="s">
+      <c r="F76" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="G76" s="7">
+      <c r="G76" s="6">
         <v>14</v>
       </c>
-      <c r="H76" s="7" t="s">
+      <c r="H76" s="6" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B77" s="8" t="s">
+      <c r="B77" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C77" s="8" t="s">
+      <c r="C77" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D77" s="7">
+      <c r="D77" s="6">
         <v>2720</v>
       </c>
-      <c r="E77" s="7">
+      <c r="E77" s="6">
         <v>2237</v>
       </c>
-      <c r="F77" s="11" t="s">
+      <c r="F77" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="G77" s="7">
+      <c r="G77" s="6">
         <v>24</v>
       </c>
-      <c r="H77" s="7" t="s">
+      <c r="H77" s="6" t="s">
         <v>52</v>
       </c>
     </row>
@@ -3262,205 +3422,205 @@
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A81" s="11" t="s">
+      <c r="A81" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B81" s="13" t="s">
+      <c r="B81" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="C81" s="14"/>
-      <c r="D81" s="7" t="s">
+      <c r="C81" s="27"/>
+      <c r="D81" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E81" s="7" t="s">
+      <c r="E81" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F81" s="15" t="s">
+      <c r="F81" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="G81" s="15" t="s">
+      <c r="G81" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="H81" s="15" t="s">
+      <c r="H81" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="I81" s="15" t="s">
+      <c r="I81" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="J81" s="15" t="s">
+      <c r="J81" s="9" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A82" s="7" t="s">
+      <c r="A82" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B82" s="13" t="s">
+      <c r="B82" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="C82" s="14"/>
-      <c r="D82" s="11">
+      <c r="C82" s="27"/>
+      <c r="D82" s="8">
         <v>2124</v>
       </c>
-      <c r="E82" s="11">
+      <c r="E82" s="8">
         <v>2235</v>
       </c>
-      <c r="F82" s="16">
+      <c r="F82" s="10">
         <f>0.2*D82+0.5*E82</f>
         <v>1542.3</v>
       </c>
-      <c r="G82" s="16">
+      <c r="G82" s="10">
         <f>F82/F87</f>
         <v>0.1947471431277227</v>
       </c>
-      <c r="H82" s="16">
+      <c r="H82" s="10">
         <f>G82</f>
         <v>0.1947471431277227</v>
       </c>
-      <c r="I82" s="16">
+      <c r="I82" s="10">
         <v>0.21197290015016035</v>
       </c>
-      <c r="J82" s="7" t="s">
+      <c r="J82" s="6" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A83" s="7" t="s">
+      <c r="A83" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B83" s="13" t="s">
+      <c r="B83" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="C83" s="14"/>
-      <c r="D83" s="11">
+      <c r="C83" s="27"/>
+      <c r="D83" s="8">
         <v>3881</v>
       </c>
-      <c r="E83" s="11">
+      <c r="E83" s="8">
         <v>1859</v>
       </c>
-      <c r="F83" s="16">
-        <f t="shared" ref="F83:F86" si="18">0.2*D83+0.5*E83</f>
+      <c r="F83" s="10">
+        <f t="shared" ref="F83:F86" si="20">0.2*D83+0.5*E83</f>
         <v>1705.7</v>
       </c>
-      <c r="G83" s="16">
+      <c r="G83" s="10">
         <f>F83/F87</f>
         <v>0.21537975882315805</v>
       </c>
-      <c r="H83" s="16">
+      <c r="H83" s="10">
         <f>H82+G83</f>
         <v>0.41012690195088075</v>
       </c>
-      <c r="I83" s="16">
+      <c r="I83" s="10">
         <v>0.99411238798091606</v>
       </c>
-      <c r="J83" s="7" t="s">
+      <c r="J83" s="6" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A84" s="7" t="s">
+      <c r="A84" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B84" s="13" t="s">
+      <c r="B84" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C84" s="14"/>
-      <c r="D84" s="11">
+      <c r="C84" s="27"/>
+      <c r="D84" s="8">
         <v>2720</v>
       </c>
-      <c r="E84" s="11">
+      <c r="E84" s="8">
         <v>2221</v>
       </c>
-      <c r="F84" s="16">
-        <f t="shared" si="18"/>
+      <c r="F84" s="10">
+        <f t="shared" si="20"/>
         <v>1654.5</v>
       </c>
-      <c r="G84" s="16">
+      <c r="G84" s="10">
         <f>F84/F87</f>
         <v>0.20891470421112443</v>
       </c>
-      <c r="H84" s="16">
+      <c r="H84" s="10">
         <f>H83+G84</f>
         <v>0.61904160616200521</v>
       </c>
-      <c r="I84" s="16">
+      <c r="I84" s="10">
         <v>0.82511539042954996</v>
       </c>
-      <c r="J84" s="7" t="s">
+      <c r="J84" s="6" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A85" s="7" t="s">
+      <c r="A85" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B85" s="13" t="s">
+      <c r="B85" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="C85" s="14"/>
-      <c r="D85" s="7">
+      <c r="C85" s="27"/>
+      <c r="D85" s="6">
         <v>2125</v>
       </c>
-      <c r="E85" s="7">
+      <c r="E85" s="6">
         <v>1859</v>
       </c>
-      <c r="F85" s="16">
-        <f t="shared" si="18"/>
+      <c r="F85" s="10">
+        <f t="shared" si="20"/>
         <v>1354.5</v>
       </c>
-      <c r="G85" s="16">
+      <c r="G85" s="10">
         <f>F85/F87</f>
         <v>0.17103352484374013</v>
       </c>
-      <c r="H85" s="16">
+      <c r="H85" s="10">
         <f>H84+G85</f>
         <v>0.79007513100574533</v>
       </c>
-      <c r="I85" s="16">
+      <c r="I85" s="10">
         <v>0.33630823824941314</v>
       </c>
-      <c r="J85" s="7" t="s">
+      <c r="J85" s="6" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A86" s="7" t="s">
+      <c r="A86" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B86" s="13" t="s">
+      <c r="B86" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="C86" s="14"/>
-      <c r="D86" s="7">
+      <c r="C86" s="27"/>
+      <c r="D86" s="6">
         <v>2720</v>
       </c>
-      <c r="E86" s="7">
+      <c r="E86" s="6">
         <v>2237</v>
       </c>
-      <c r="F86" s="16">
-        <f t="shared" si="18"/>
+      <c r="F86" s="10">
+        <f t="shared" si="20"/>
         <v>1662.5</v>
       </c>
-      <c r="G86" s="16">
+      <c r="G86" s="10">
         <f>F86/F87</f>
         <v>0.20992486899425469</v>
       </c>
-      <c r="H86" s="16">
+      <c r="H86" s="10">
         <f>H85+G86</f>
         <v>1</v>
       </c>
-      <c r="I86" s="16">
+      <c r="I86" s="10">
         <v>0.43910472544948531</v>
       </c>
-      <c r="J86" s="7" t="s">
+      <c r="J86" s="6" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E87" s="7" t="s">
+      <c r="E87" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F87" s="16">
+      <c r="F87" s="10">
         <f>SUM(F82:F86)</f>
         <v>7919.5</v>
       </c>
@@ -3471,377 +3631,377 @@
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A92" s="7" t="s">
+      <c r="A92" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B92" s="6" t="s">
+      <c r="B92" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C92" s="6"/>
-      <c r="D92" s="7" t="s">
+      <c r="C92" s="35"/>
+      <c r="D92" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E92" s="7" t="s">
+      <c r="E92" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F92" s="7" t="s">
+      <c r="F92" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G92" s="7" t="s">
+      <c r="G92" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H92" s="7" t="s">
+      <c r="H92" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I92" s="7" t="s">
+      <c r="I92" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J92" s="7" t="s">
+      <c r="J92" s="6" t="s">
         <v>28</v>
       </c>
       <c r="L92" t="s">
         <v>65</v>
       </c>
-      <c r="M92" s="18" t="s">
+      <c r="M92" s="12" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A93" s="7" t="s">
+      <c r="A93" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B93" s="19" t="s">
+      <c r="B93" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="C93" s="14"/>
-      <c r="D93" s="11">
+      <c r="C93" s="27"/>
+      <c r="D93" s="8">
         <v>3881</v>
       </c>
-      <c r="E93" s="11">
+      <c r="E93" s="8">
         <v>1859</v>
       </c>
-      <c r="F93" s="7" t="str">
+      <c r="F93" s="6" t="str">
         <f>IF(0.1*D93+0.6*E93&lt;=2000,"T","F")</f>
         <v>T</v>
       </c>
-      <c r="G93" s="7" t="str">
+      <c r="G93" s="6" t="str">
         <f>IF(D93+E93&lt;=6000,"T","F")</f>
         <v>T</v>
       </c>
-      <c r="H93" s="7" t="str">
+      <c r="H93" s="6" t="str">
         <f>IF(D93&lt;=4000,"T","F")</f>
         <v>T</v>
       </c>
-      <c r="I93" s="7" t="str">
+      <c r="I93" s="6" t="str">
         <f>IF(D93&gt;=0,"T","F")</f>
         <v>T</v>
       </c>
-      <c r="J93" s="7" t="str">
+      <c r="J93" s="6" t="str">
         <f>IF(E93&gt;=0,"T","F")</f>
         <v>T</v>
       </c>
       <c r="L93" t="str">
         <f ca="1">IF(RAND()*10&gt;5,"Mutación","Cruce")</f>
-        <v>Cruce</v>
-      </c>
-      <c r="M93" s="17">
+        <v>Mutación</v>
+      </c>
+      <c r="M93" s="11">
         <f ca="1">RAND()*27</f>
-        <v>3.4364352589063141</v>
+        <v>0.28465771775272819</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A94" s="7" t="s">
+      <c r="A94" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B94" s="19" t="s">
+      <c r="B94" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C94" s="14"/>
-      <c r="D94" s="11">
+      <c r="C94" s="27"/>
+      <c r="D94" s="8">
         <v>2720</v>
       </c>
-      <c r="E94" s="11">
+      <c r="E94" s="8">
         <v>2221</v>
       </c>
-      <c r="F94" s="7" t="str">
-        <f t="shared" ref="F94:F97" si="19">IF(0.1*D94+0.6*E94&lt;=2000,"T","F")</f>
-        <v>T</v>
-      </c>
-      <c r="G94" s="7" t="str">
-        <f t="shared" ref="G94:G97" si="20">IF(D94+E94&lt;=6000,"T","F")</f>
-        <v>T</v>
-      </c>
-      <c r="H94" s="7" t="str">
-        <f t="shared" ref="H94:H97" si="21">IF(D94&lt;=4000,"T","F")</f>
-        <v>T</v>
-      </c>
-      <c r="I94" s="7" t="str">
-        <f t="shared" ref="I94:I97" si="22">IF(D94&gt;=0,"T","F")</f>
-        <v>T</v>
-      </c>
-      <c r="J94" s="7" t="str">
-        <f t="shared" ref="J94:J97" si="23">IF(E94&gt;=0,"T","F")</f>
-        <v>T</v>
-      </c>
-      <c r="M94" s="17"/>
+      <c r="F94" s="6" t="str">
+        <f t="shared" ref="F94:F97" si="21">IF(0.1*D94+0.6*E94&lt;=2000,"T","F")</f>
+        <v>T</v>
+      </c>
+      <c r="G94" s="6" t="str">
+        <f t="shared" ref="G94:G97" si="22">IF(D94+E94&lt;=6000,"T","F")</f>
+        <v>T</v>
+      </c>
+      <c r="H94" s="6" t="str">
+        <f t="shared" ref="H94:H97" si="23">IF(D94&lt;=4000,"T","F")</f>
+        <v>T</v>
+      </c>
+      <c r="I94" s="6" t="str">
+        <f t="shared" ref="I94:I97" si="24">IF(D94&gt;=0,"T","F")</f>
+        <v>T</v>
+      </c>
+      <c r="J94" s="6" t="str">
+        <f t="shared" ref="J94:J97" si="25">IF(E94&gt;=0,"T","F")</f>
+        <v>T</v>
+      </c>
+      <c r="M94" s="11"/>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A95" s="7" t="s">
+      <c r="A95" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B95" s="19" t="s">
+      <c r="B95" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="C95" s="14"/>
-      <c r="D95" s="7">
+      <c r="C95" s="27"/>
+      <c r="D95" s="6">
         <v>2720</v>
       </c>
-      <c r="E95" s="7">
+      <c r="E95" s="6">
         <v>2237</v>
       </c>
-      <c r="F95" s="7" t="str">
-        <f t="shared" si="19"/>
-        <v>T</v>
-      </c>
-      <c r="G95" s="7" t="str">
-        <f t="shared" si="20"/>
-        <v>T</v>
-      </c>
-      <c r="H95" s="7" t="str">
+      <c r="F95" s="6" t="str">
         <f t="shared" si="21"/>
         <v>T</v>
       </c>
-      <c r="I95" s="7" t="str">
+      <c r="G95" s="6" t="str">
         <f t="shared" si="22"/>
         <v>T</v>
       </c>
-      <c r="J95" s="7" t="str">
+      <c r="H95" s="6" t="str">
         <f t="shared" si="23"/>
         <v>T</v>
       </c>
+      <c r="I95" s="6" t="str">
+        <f t="shared" si="24"/>
+        <v>T</v>
+      </c>
+      <c r="J95" s="6" t="str">
+        <f t="shared" si="25"/>
+        <v>T</v>
+      </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A96" s="7" t="s">
+      <c r="A96" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B96" s="19" t="s">
+      <c r="B96" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="C96" s="14"/>
-      <c r="D96" s="7">
-        <f t="shared" ref="D96:E96" si="24">D104</f>
+      <c r="C96" s="27"/>
+      <c r="D96" s="6">
+        <f t="shared" ref="D96:E96" si="26">D104</f>
         <v>1548</v>
       </c>
-      <c r="E96" s="7">
+      <c r="E96" s="6">
+        <f t="shared" si="26"/>
+        <v>2235</v>
+      </c>
+      <c r="F96" s="6" t="str">
+        <f t="shared" si="21"/>
+        <v>T</v>
+      </c>
+      <c r="G96" s="6" t="str">
+        <f t="shared" si="22"/>
+        <v>T</v>
+      </c>
+      <c r="H96" s="6" t="str">
+        <f t="shared" si="23"/>
+        <v>T</v>
+      </c>
+      <c r="I96" s="6" t="str">
         <f t="shared" si="24"/>
-        <v>2235</v>
-      </c>
-      <c r="F96" s="7" t="str">
-        <f t="shared" si="19"/>
-        <v>T</v>
-      </c>
-      <c r="G96" s="7" t="str">
-        <f t="shared" si="20"/>
-        <v>T</v>
-      </c>
-      <c r="H96" s="7" t="str">
+        <v>T</v>
+      </c>
+      <c r="J96" s="6" t="str">
+        <f t="shared" si="25"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A97" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B97" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C97" s="27"/>
+      <c r="D97" s="6">
+        <f t="shared" ref="D97:E97" si="27">D105</f>
+        <v>2728</v>
+      </c>
+      <c r="E97" s="6">
+        <f t="shared" si="27"/>
+        <v>2221</v>
+      </c>
+      <c r="F97" s="6" t="str">
         <f t="shared" si="21"/>
         <v>T</v>
       </c>
-      <c r="I96" s="7" t="str">
+      <c r="G97" s="6" t="str">
         <f t="shared" si="22"/>
         <v>T</v>
       </c>
-      <c r="J96" s="7" t="str">
+      <c r="H97" s="6" t="str">
         <f t="shared" si="23"/>
         <v>T</v>
       </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A97" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B97" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="C97" s="14"/>
-      <c r="D97" s="7">
-        <f t="shared" ref="D97:E97" si="25">D105</f>
-        <v>2728</v>
-      </c>
-      <c r="E97" s="7">
+      <c r="I97" s="6" t="str">
+        <f t="shared" si="24"/>
+        <v>T</v>
+      </c>
+      <c r="J97" s="6" t="str">
         <f t="shared" si="25"/>
-        <v>2221</v>
-      </c>
-      <c r="F97" s="7" t="str">
-        <f t="shared" si="19"/>
-        <v>T</v>
-      </c>
-      <c r="G97" s="7" t="str">
-        <f t="shared" si="20"/>
-        <v>T</v>
-      </c>
-      <c r="H97" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v>T</v>
-      </c>
-      <c r="I97" s="7" t="str">
-        <f t="shared" si="22"/>
-        <v>T</v>
-      </c>
-      <c r="J97" s="7" t="str">
-        <f t="shared" si="23"/>
         <v>T</v>
       </c>
       <c r="L97" s="1"/>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B99" s="6" t="s">
+      <c r="B99" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C99" s="6"/>
-      <c r="D99" s="6" t="s">
+      <c r="C99" s="35"/>
+      <c r="D99" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E99" s="6"/>
-      <c r="F99" s="12" t="s">
+      <c r="E99" s="35"/>
+      <c r="F99" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="G99" s="12" t="s">
+      <c r="G99" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="H99" s="20" t="s">
+      <c r="H99" s="31" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B100" s="7" t="s">
+      <c r="B100" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C100" s="7" t="s">
+      <c r="C100" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D100" s="7" t="s">
+      <c r="D100" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E100" s="7" t="s">
+      <c r="E100" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F100" s="12"/>
-      <c r="G100" s="12"/>
-      <c r="H100" s="20"/>
+      <c r="F100" s="30"/>
+      <c r="G100" s="30"/>
+      <c r="H100" s="31"/>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B101" s="8" t="s">
+      <c r="B101" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C101" s="8" t="s">
+      <c r="C101" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D101" s="7">
+      <c r="D101" s="6">
         <v>1546</v>
       </c>
-      <c r="E101" s="7">
+      <c r="E101" s="6">
         <v>1316</v>
       </c>
-      <c r="F101" s="11" t="s">
+      <c r="F101" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="G101" s="21" t="s">
+      <c r="G101" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="H101" s="22"/>
+      <c r="H101" s="14"/>
       <c r="I101" s="4"/>
       <c r="J101" s="4"/>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B102" s="8" t="s">
+      <c r="B102" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C102" s="8" t="s">
+      <c r="C102" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D102" s="7">
+      <c r="D102" s="6">
         <v>2124</v>
       </c>
-      <c r="E102" s="7">
+      <c r="E102" s="6">
         <v>2235</v>
       </c>
-      <c r="F102" s="11" t="s">
+      <c r="F102" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="G102" s="21" t="s">
+      <c r="G102" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="H102" s="22"/>
+      <c r="H102" s="14"/>
       <c r="I102" s="4"/>
       <c r="J102" s="4"/>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B103" s="8" t="s">
+      <c r="B103" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C103" s="8" t="s">
+      <c r="C103" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D103" s="7">
+      <c r="D103" s="6">
         <v>2720</v>
       </c>
-      <c r="E103" s="7">
+      <c r="E103" s="6">
         <v>2237</v>
       </c>
-      <c r="F103" s="11" t="s">
+      <c r="F103" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="G103" s="11" t="s">
+      <c r="G103" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="H103" s="7"/>
+      <c r="H103" s="6"/>
       <c r="L103" s="1"/>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B104" s="8" t="s">
+      <c r="B104" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C104" s="8" t="s">
+      <c r="C104" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D104" s="7">
+      <c r="D104" s="6">
         <v>1548</v>
       </c>
-      <c r="E104" s="7">
+      <c r="E104" s="6">
         <v>2235</v>
       </c>
-      <c r="F104" s="11" t="s">
+      <c r="F104" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="G104" s="7">
+      <c r="G104" s="6">
         <v>10</v>
       </c>
-      <c r="H104" s="7" t="s">
+      <c r="H104" s="6" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B105" s="8" t="s">
+      <c r="B105" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C105" s="8" t="s">
+      <c r="C105" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D105" s="7">
+      <c r="D105" s="6">
         <v>2728</v>
       </c>
-      <c r="E105" s="7">
+      <c r="E105" s="6">
         <v>2221</v>
       </c>
-      <c r="F105" s="11" t="s">
+      <c r="F105" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="G105" s="7">
+      <c r="G105" s="6">
         <v>12</v>
       </c>
-      <c r="H105" s="7" t="s">
+      <c r="H105" s="6" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3851,235 +4011,235 @@
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A109" s="11" t="s">
+      <c r="A109" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B109" s="13" t="s">
+      <c r="B109" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="C109" s="14"/>
-      <c r="D109" s="7" t="s">
+      <c r="C109" s="27"/>
+      <c r="D109" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E109" s="7" t="s">
+      <c r="E109" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F109" s="15" t="s">
+      <c r="F109" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="G109" s="15" t="s">
+      <c r="G109" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="H109" s="15" t="s">
+      <c r="H109" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="I109" s="15" t="s">
+      <c r="I109" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="J109" s="15" t="s">
+      <c r="J109" s="9" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A110" s="29" t="s">
+      <c r="A110" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="B110" s="30" t="s">
+      <c r="B110" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="C110" s="31"/>
-      <c r="D110" s="15">
+      <c r="C110" s="34"/>
+      <c r="D110" s="9">
         <v>3881</v>
       </c>
-      <c r="E110" s="15">
+      <c r="E110" s="9">
         <v>1859</v>
       </c>
-      <c r="F110" s="32">
+      <c r="F110" s="22">
         <f>0.2*D110+0.5*E110</f>
         <v>1705.7</v>
       </c>
-      <c r="G110" s="32">
+      <c r="G110" s="22">
         <f>F110/F115</f>
         <v>0.2104269729456322</v>
       </c>
-      <c r="H110" s="32">
+      <c r="H110" s="22">
         <f>G110</f>
         <v>0.2104269729456322</v>
       </c>
-      <c r="I110" s="32">
+      <c r="I110" s="22">
         <v>0.2595844651573761</v>
       </c>
-      <c r="J110" s="29" t="s">
+      <c r="J110" s="21" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A111" s="7" t="s">
+      <c r="A111" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B111" s="19" t="s">
+      <c r="B111" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C111" s="14"/>
-      <c r="D111" s="11">
+      <c r="C111" s="27"/>
+      <c r="D111" s="8">
         <v>2720</v>
       </c>
-      <c r="E111" s="11">
+      <c r="E111" s="8">
         <v>2221</v>
       </c>
-      <c r="F111" s="16">
-        <f t="shared" ref="F111:F114" si="26">0.2*D111+0.5*E111</f>
+      <c r="F111" s="10">
+        <f t="shared" ref="F111:F114" si="28">0.2*D111+0.5*E111</f>
         <v>1654.5</v>
       </c>
-      <c r="G111" s="16">
+      <c r="G111" s="10">
         <f>F111/F115</f>
         <v>0.20411058611628569</v>
       </c>
-      <c r="H111" s="16">
+      <c r="H111" s="10">
         <f>H110+G111</f>
         <v>0.41453755906191792</v>
       </c>
-      <c r="I111" s="16">
+      <c r="I111" s="10">
         <v>0.50122092908795157</v>
       </c>
-      <c r="J111" s="7" t="s">
+      <c r="J111" s="6" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A112" s="33" t="s">
+      <c r="A112" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="B112" s="34" t="s">
+      <c r="B112" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="C112" s="35"/>
-      <c r="D112" s="33">
+      <c r="C112" s="29"/>
+      <c r="D112" s="23">
         <v>2720</v>
       </c>
-      <c r="E112" s="33">
+      <c r="E112" s="23">
         <v>2237</v>
       </c>
-      <c r="F112" s="36">
-        <f t="shared" si="26"/>
+      <c r="F112" s="24">
+        <f t="shared" si="28"/>
         <v>1662.5</v>
       </c>
-      <c r="G112" s="36">
+      <c r="G112" s="24">
         <f>F112/F115</f>
         <v>0.20509752155837108</v>
       </c>
-      <c r="H112" s="36">
+      <c r="H112" s="24">
         <f>H111+G112</f>
         <v>0.61963508062028905</v>
       </c>
-      <c r="I112" s="36">
+      <c r="I112" s="24">
         <v>0.21554893216354676</v>
       </c>
-      <c r="J112" s="33" t="s">
+      <c r="J112" s="23" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A113" s="7" t="s">
+      <c r="A113" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B113" s="19" t="s">
+      <c r="B113" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="C113" s="14"/>
-      <c r="D113" s="7">
+      <c r="C113" s="27"/>
+      <c r="D113" s="6">
         <v>1548</v>
       </c>
-      <c r="E113" s="7">
+      <c r="E113" s="6">
         <v>2235</v>
       </c>
-      <c r="F113" s="16">
-        <f t="shared" si="26"/>
+      <c r="F113" s="10">
+        <f t="shared" si="28"/>
         <v>1427.1</v>
       </c>
-      <c r="G113" s="16">
+      <c r="G113" s="10">
         <f>F113/F115</f>
         <v>0.17605694617500833</v>
       </c>
-      <c r="H113" s="16">
+      <c r="H113" s="10">
         <f>H112+G113</f>
         <v>0.79569202679529738</v>
       </c>
-      <c r="I113" s="16">
+      <c r="I113" s="10">
         <v>0.43710054322453973</v>
       </c>
-      <c r="J113" s="7" t="s">
+      <c r="J113" s="6" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A114" s="7" t="s">
+      <c r="A114" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B114" s="19" t="s">
+      <c r="B114" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="C114" s="14"/>
-      <c r="D114" s="7">
+      <c r="C114" s="27"/>
+      <c r="D114" s="6">
         <v>2728</v>
       </c>
-      <c r="E114" s="7">
+      <c r="E114" s="6">
         <v>2221</v>
       </c>
-      <c r="F114" s="16">
-        <f t="shared" si="26"/>
+      <c r="F114" s="10">
+        <f t="shared" si="28"/>
         <v>1656.1</v>
       </c>
-      <c r="G114" s="16">
+      <c r="G114" s="10">
         <f>F114/F115</f>
         <v>0.20430797320470276</v>
       </c>
-      <c r="H114" s="16">
+      <c r="H114" s="10">
         <f>H113+G114</f>
         <v>1.0000000000000002</v>
       </c>
-      <c r="I114" s="16">
+      <c r="I114" s="10">
         <v>0.74044162752641896</v>
       </c>
-      <c r="J114" s="7" t="s">
+      <c r="J114" s="6" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E115" s="7" t="s">
+      <c r="E115" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F115" s="16">
+      <c r="F115" s="10">
         <f>SUM(F110:F114)</f>
         <v>8105.9</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A117" s="23" t="s">
+      <c r="A117" s="15" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A118" s="37" t="s">
+      <c r="A118" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B118" s="37">
+      <c r="B118" s="25">
         <v>2720</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A119" s="37" t="s">
+      <c r="A119" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B119" s="37">
+      <c r="B119" s="25">
         <v>2237</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A120" s="37" t="s">
+      <c r="A120" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B120" s="37">
+      <c r="B120" s="25">
         <v>1662.5</v>
       </c>
     </row>
@@ -4089,36 +4249,64 @@
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A123" s="37" t="s">
+      <c r="A123" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B123" s="37">
+      <c r="B123" s="25">
         <v>3200</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A124" s="37" t="s">
+      <c r="A124" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B124" s="37">
+      <c r="B124" s="25">
         <v>2800</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A125" s="37" t="s">
+      <c r="A125" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B125" s="37">
+      <c r="B125" s="25">
         <v>2040</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="F99:F100"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:F72"/>
+    <mergeCell ref="G71:G72"/>
+    <mergeCell ref="H71:H72"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="B92:C92"/>
     <mergeCell ref="G99:G100"/>
     <mergeCell ref="H99:H100"/>
     <mergeCell ref="B109:C109"/>
@@ -4129,39 +4317,11 @@
     <mergeCell ref="B97:C97"/>
     <mergeCell ref="B99:C99"/>
     <mergeCell ref="D99:E99"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="B93:C93"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:F72"/>
-    <mergeCell ref="G71:G72"/>
-    <mergeCell ref="H71:H72"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="F99:F100"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4169,7 +4329,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -4254,30 +4414,30 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="17" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="27">
+      <c r="D16" s="19">
         <v>0</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="19">
         <v>2040</v>
       </c>
     </row>
@@ -4287,53 +4447,53 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="E20" s="25" t="s">
+      <c r="E20" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="F20" s="25" t="s">
+      <c r="F20" s="17" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="28">
+      <c r="D21" s="20">
         <v>0</v>
       </c>
-      <c r="E21" s="28">
+      <c r="E21" s="20">
         <v>3199.9999999999991</v>
       </c>
-      <c r="F21" s="26" t="s">
+      <c r="F21" s="18" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="27">
+      <c r="D22" s="19">
         <v>0</v>
       </c>
-      <c r="E22" s="27">
+      <c r="E22" s="19">
         <v>2800</v>
       </c>
-      <c r="F22" s="24" t="s">
+      <c r="F22" s="16" t="s">
         <v>115</v>
       </c>
     </row>
@@ -4343,82 +4503,82 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="D26" s="25" t="s">
+      <c r="D26" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="E26" s="25" t="s">
+      <c r="E26" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="F26" s="25" t="s">
+      <c r="F26" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="G26" s="25" t="s">
+      <c r="G26" s="17" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="D27" s="28">
+      <c r="D27" s="20">
         <v>2000</v>
       </c>
-      <c r="E27" s="26" t="s">
+      <c r="E27" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="F27" s="26" t="s">
+      <c r="F27" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="G27" s="26">
+      <c r="G27" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="D28" s="28">
+      <c r="D28" s="20">
         <v>5999.9999999999991</v>
       </c>
-      <c r="E28" s="26" t="s">
+      <c r="E28" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="F28" s="26" t="s">
+      <c r="F28" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="G28" s="26">
+      <c r="G28" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C29" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="D29" s="27">
+      <c r="D29" s="19">
         <v>3199.9999999999991</v>
       </c>
-      <c r="E29" s="24" t="s">
+      <c r="E29" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="F29" s="24" t="s">
+      <c r="F29" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="G29" s="24">
+      <c r="G29" s="16">
         <v>800.00000000000091</v>
       </c>
     </row>
@@ -4428,7 +4588,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>